<commit_message>
updated readme about importing strings from CSV
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -529,7 +529,7 @@
     <t>在线图书馆卡登记表</t>
   </si>
   <si>
-    <t>As parent/Legal Guardian, I understand and agree that:&lt;br /&gt;&lt;ul&gt;&lt;li&gt;The library may only give the card to my child.  Only my child may use his or her card.&lt;/li&gt;&lt;li&gt;The library allows my child to use any materials, from any section.   The library cannot limit the types of books or movies my child checks out, even if I ask.&lt;/li&gt;&lt;li&gt;My child’s library record (like mine) is private by law. The library cannot tell me what my child has checked out, except when a fine is owed.&lt;/li&gt;&lt;li&gt;Some materials have fines if they are returned late, and all lost or damaged materials have fines.  I am responsible for any fines on my child’s record.&lt;/li&gt;&lt;li&gt;My child can use computers at the library for up to one hour per day.  The library does not limit what children can look at, and does not supervise children on the computer.&lt;/li&gt;&lt;li&gt;If my child is younger than eight years old, he or she must be closely supervised by a parent or responsible caregiver, and may not be left unattended in the library.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>As parent/Legal Guardian, I understand and agree that:&lt;br /&gt;&lt;ul&gt;&lt;li&gt;The library may only give the card to my child.  Only my child may use his or her card.&lt;/li&gt;&lt;li&gt;The library allows my child to use any materials, from any section. The library cannot limit the types of books or movies my child checks out, even if I ask.&lt;/li&gt;&lt;li&gt;My child's library record (like mine) is private by law. The library cannot tell me what my child has checked out, except when a fine is owed.&lt;/li&gt;&lt;li&gt;Some materials have fines if they are returned late, and all lost or damaged materials have fines. I am responsible for any fines on my child's record.&lt;/li&gt;&lt;li&gt;My child can use computers at the library for up to one hour per day. The library does not limit what children can look at, and does not supervise children on the computer.&lt;/li&gt;&lt;li&gt;If my child is younger than eight years old, he or she must be closely supervised by a parent or responsible caregiver, and may not be left unattended in the library.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -1364,14 +1364,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
updated spreadsheet, still need some chinese and spanish translations
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="token_data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="token_data" localSheetId="0">token_data!$A$1:$D$82</definedName>
+    <definedName name="token_data" localSheetId="0">token_data!$A$1:$D$81</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="246">
   <si>
     <t>header</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Please Enter Your Birth Date</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>header_adult</t>
   </si>
   <si>
@@ -304,12 +298,6 @@
     <t>School</t>
   </si>
   <si>
-    <t>parent_note</t>
-  </si>
-  <si>
-    <t>You may register using one of several identification types. Please select an identification type by clicking one of the buttons below, and then enter the number shown on your ID. For more information about the accepted types of identification, please see &amp;ldquo;&lt;a href="#" onclick="lightbox_open(acceptable_id());"&gt;What forms of identification are accepted?&lt;/a&gt;&amp;rdquo;</t>
-  </si>
-  <si>
     <t>ident</t>
   </si>
   <si>
@@ -394,9 +382,6 @@
     <t>submit_error</t>
   </si>
   <si>
-    <t>Submission Error</t>
-  </si>
-  <si>
     <t>submit_error_note</t>
   </si>
   <si>
@@ -517,26 +502,720 @@
     <t>Print Confirmation</t>
   </si>
   <si>
-    <t>button_startover</t>
-  </si>
-  <si>
     <t>Close</t>
   </si>
   <si>
     <t>Formulario de Inscripción Card Library Online</t>
   </si>
   <si>
-    <t>在线图书馆卡登记表</t>
-  </si>
-  <si>
     <t>As parent/Legal Guardian, I understand and agree that:&lt;br /&gt;&lt;ul&gt;&lt;li&gt;The library may only give the card to my child.  Only my child may use his or her card.&lt;/li&gt;&lt;li&gt;The library allows my child to use any materials, from any section. The library cannot limit the types of books or movies my child checks out, even if I ask.&lt;/li&gt;&lt;li&gt;My child's library record (like mine) is private by law. The library cannot tell me what my child has checked out, except when a fine is owed.&lt;/li&gt;&lt;li&gt;Some materials have fines if they are returned late, and all lost or damaged materials have fines. I am responsible for any fines on my child's record.&lt;/li&gt;&lt;li&gt;My child can use computers at the library for up to one hour per day. The library does not limit what children can look at, and does not supervise children on the computer.&lt;/li&gt;&lt;li&gt;If my child is younger than eight years old, he or she must be closely supervised by a parent or responsible caregiver, and may not be left unattended in the library.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Error Submitting Form</t>
+  </si>
+  <si>
+    <t>網上圖書証申請表</t>
+  </si>
+  <si>
+    <t>請填寫你的出生日期</t>
+  </si>
+  <si>
+    <t>如果你是殘障人士，請向圖書館職員索取殘障讀者專用特別服務申請表。</t>
+  </si>
+  <si>
+    <t>必須填寫項目</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>姓</t>
+  </si>
+  <si>
+    <t>名</t>
+  </si>
+  <si>
+    <t>中間名簡寫</t>
+  </si>
+  <si>
+    <t>住所地址</t>
+  </si>
+  <si>
+    <t>街名</t>
+  </si>
+  <si>
+    <t>房號</t>
+  </si>
+  <si>
+    <t>巿名</t>
+  </si>
+  <si>
+    <t>郵區號碼</t>
+  </si>
+  <si>
+    <t>電話</t>
+  </si>
+  <si>
+    <t>包括地區號碼</t>
+  </si>
+  <si>
+    <t>電郵地址</t>
+  </si>
+  <si>
+    <t>首選語言</t>
+  </si>
+  <si>
+    <t>若你選擇閱讀英文以外的語文，請在這裏填寫</t>
+  </si>
+  <si>
+    <t>個人識別號碼</t>
+  </si>
+  <si>
+    <t>証件號碼</t>
+  </si>
+  <si>
+    <t>網上同意書</t>
+  </si>
+  <si>
+    <t>本人同意遵守所有圖書館的規定</t>
+  </si>
+  <si>
+    <t>重新開始</t>
+  </si>
+  <si>
+    <t>青少年圖書証申請表</t>
+  </si>
+  <si>
+    <t>學校</t>
+  </si>
+  <si>
+    <t>作為家長/監護人我明白及同意&lt;br/&gt;&lt;ul&gt;&lt;li&gt;圖書館只發証給我的孩子，只有我的孩子才能使用這張圖書証。&lt;/li&gt;&lt;li&gt;圖書館容許孩子從任何部份借出任何物件。即使在本人的要求下，圖書館不能限制孩子借出書本及電影的種類。&lt;/li&gt;&lt;li&gt;孩子的資料保密與本人一樣是受加州私隱權法例保障的。圖書館不可向我透露孩子借出的任何資料，除物件有罰款以外。&lt;/li&gt;&lt;li&gt;某些圖書館物件是有過期罰款的。所有遺失及損壞物件均需繳付費用。本人同意對孩子借出的一切物件負責，並擔負所有過期罰款及任何損壞費用。&lt;/li&gt;&lt;li&gt;我的孩子每天只可在圖書館內使用不超過一小時的電腦 圖書館不會監察孩子在網上查閱的任何資料。&lt;/li&gt;&lt;li&gt;若我的孩子年齡是八歲以下，必須時刻由家長或保姆監督，絶不可以單獨逗留在圖書館內。&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>button_close</t>
+  </si>
+  <si>
+    <r>
+      <t>Registró</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para tarjetas de la biblioteca para adultos (personas de 18 años o más)</t>
+    </r>
+  </si>
+  <si>
+    <t>Recoja su tarjeta de la biblioteca en persona en su sucursal más cercano en los próximos 14 días y traiga los siguientes documentos:&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Identificación fotográfica&lt;/li&gt;&lt;li&gt;Prueba de su dirección actual&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>información necesaria</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre </t>
+  </si>
+  <si>
+    <t>Inicial media</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calle con número </t>
+  </si>
+  <si>
+    <t>Apt. #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciudad </t>
+  </si>
+  <si>
+    <t>CA Código postal</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>(incluya código de área)</t>
+  </si>
+  <si>
+    <t>Dirección para correspondencia (solo si se diferente al de su casa)</t>
+  </si>
+  <si>
+    <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idioma preferido </t>
+  </si>
+  <si>
+    <t>Si usted prefiere leer en otro idioma que no sea inglés, favor de indicarlo</t>
+  </si>
+  <si>
+    <t>Usted se puede registrar usando uno de varios tipos de identificación. Favor de indicar cual tipo de identificación desea usar y ponga el numero abajo. Para más información acerca de cuales tipos de identificación son aceptados vea &amp;ldquo;&lt;a href="#" onclick="lightbox_open(acceptable_id());"&gt;What forms of identification are accepted?&lt;/a&gt;&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>Licencia de conducir</t>
+  </si>
+  <si>
+    <t>Tarjeta verde ( Tarjeta de residencia permanente)</t>
+  </si>
+  <si>
+    <t>Identificación estatal</t>
+  </si>
+  <si>
+    <t>Matricula consular</t>
+  </si>
+  <si>
+    <t>Identificación de la Ciudad de Oakland</t>
+  </si>
+  <si>
+    <t>Identificación escolar</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numero de su identificación </t>
+  </si>
+  <si>
+    <t>Acepto seguir todas las reglas de la biblioteca, pagar todos los cargos y multas y notificar cambios de domicilio, teléfono o si se extravía me tarjeta.  Entiendo que soy responsable por todos los materiales que se prestan con mi tarjeta, que algunos materiales tales como videos y DVD tienen multas más altas y que yo soy la única persona autorizada para usar esta tarjeta.</t>
+  </si>
+  <si>
+    <t>Yo acepto seguir todas las reglas.</t>
+  </si>
+  <si>
+    <t>Continúe</t>
+  </si>
+  <si>
+    <t>Empezar de nuevo</t>
+  </si>
+  <si>
+    <t>Recoja su tarjeta de la biblioteca en persona en su sucursal más cercano en los próximos 14 días y traiga identificación fotográfica.</t>
+  </si>
+  <si>
+    <t>Padres de familia/ guardián y el niño tiene que presentase para recibir la tarjeta en los próximos 14 días. O, pueden imprimir y completar la solicitud y el niño puede recibir su tarjecta sin que estén presente los padres/ guardián.</t>
+  </si>
+  <si>
+    <t>Escuela</t>
+  </si>
+  <si>
+    <t>Padre / guardia</t>
+  </si>
+  <si>
+    <t>Acuerdo en línea</t>
+  </si>
+  <si>
+    <t>Como padre de familia/ guardián acepto las siguientes responsabilidades:&lt;br/&gt;&lt;ul&gt;&lt;li&gt;La biblioteca puede darle solamente a mi niño la tarjecta. Solo mi niño puede usar su tarjects.&lt;/li&gt;&lt;li&gt;La biblioteca permite que mi niño use cualquier material de cualquier sección.  La biblioteca no puede limitar el tipo de libros o películas que mi niño puede sacar aun si yo lo pido&lt;/li&gt;&lt;li&gt;La cuenta de mi niño (al igual que la mía) es privada bajo la ley. La biblioteca no me puede dar información acerca de lo que esta prestado a mi niño a menos que sea acerca de las multas.&lt;/li&gt;&lt;li&gt;Algunos materiales tiene multas si se regresan tarde y siempre hay cargos si material se pierde o regresa dañado. Yo soy responsable de todos cargos en la cuenta de mi niño.&lt;/li&gt;&lt;li&gt;Mi niño puede usar la computadora en la biblioteca hasta el máximo de una hora por día. La biblioteca no limita lo que los niños pueden ver y no supervisan a los niños en la computadora.&lt;/li&gt;&lt;li&gt;Si mi niño es menor de 8 años debe de tener supervisión de parte de un padre u otro adulto responsable, y no puede  estar en la biblioteca solo.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Número de su identificación</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Registro para tarjeta infantil de la biblioteca</t>
+  </si>
+  <si>
+    <t>Registro para tarjetas del la biblioteca para adolescentes</t>
+  </si>
+  <si>
+    <r>
+      <t>成人圖書証申請表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>十八歲或以上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>兒童圖書証申請表</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF231F20"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF231F20"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5 - 12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF231F20"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 歲)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>提交</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Si usted es una persona con discapacidades, pida  la SOLICITUD de Servicios Extra </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Para Usuarios con Discapacidades.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>請在填寫表格後十四日內，由本人帶同以下文件到附近圖書館分館領取你的圖書証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:&lt;ol&gt;&lt;li&gt;附有照片的身份証&lt;/li&gt;&lt;li&gt;地址証明&lt;/li&gt;&lt;/ol&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>請在填寫表格後十四日內，帶同附有照片的身份証到附近圖書館分館領取你的圖書証。若不能提供身份証明文件，請填寫由家長</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>法定監護人簽名的</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>書面申請表格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>家長</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>法定監護人和孩子在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>填寫申請表格後十四日內</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，必須一同前往圖書館</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF444444"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>領取孩子的圖書証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。家長</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>法定監護人亦可預先填寫</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>書面申請表格</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>讓孩子在沒有家表的陪同下仍可辨理申請手續。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>通信地址</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (若與住所地址不同)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>家長</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>法定監護人資料</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>你可選擇使用任何一種身份証明文件申請圖書証。請點擊以下按鈕，然後輸入証件上的號碼。有關可接受的身份証種類詳情，請參閱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>駕駛執照</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>永久居民身份証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>州政府簽發身份証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>駐美墨西哥領事館簽發身份証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>屋崙市</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>或其他市政府簽發身份証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>學生証</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>護照</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>本人同意遵守圖書館的規定，支付所有遺失及受損物件的費用。若我的地址、電話有任何變動，或遺失圖書証時會立刻通知館方。我本人了解必須為所有這張圖書証借出的物件負責，包括罰款較高的錄影帶及</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>DVD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+      </rPr>
+      <t>。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>而且明白本人是這張圖書証的唯一授權使用人。</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,6 +1350,61 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF231F20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF231F20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="SimSun"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1362,18 +2096,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,10 +2118,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,1133 +2132,1120 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>227</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>216</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>47</v>
-      </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>231</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>218</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>219</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>189</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>194</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>195</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
+        <v>196</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
+        <v>199</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>202</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>203</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>4</v>
+        <v>221</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>224</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>207</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>208</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>209</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>210</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>211</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>212</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>5</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>222</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>214</v>
       </c>
       <c r="D56" t="s">
-        <v>5</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>223</v>
       </c>
       <c r="D57" t="s">
-        <v>5</v>
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>215</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D59" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D61" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D63" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C64" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D64" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C70" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D71" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D72" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C73" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D73" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D74" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D75" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C77" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C78" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D78" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C79" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C80" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D80" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C81" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="D81" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>161</v>
-      </c>
-      <c r="B82" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" t="s">
-        <v>5</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more language tokens, beginning to implement language switching
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="261">
   <si>
     <t>header</t>
   </si>
@@ -364,9 +364,6 @@
     <t>Online Agreement</t>
   </si>
   <si>
-    <t>agreement_note_adult_teen_adult</t>
-  </si>
-  <si>
     <t>I agree to follow all library rules, pay all fines and fees, and give immediate notice of any change of address, phone number, or loss of library card. I understand that I am responsible for all items checked out on this card, that some items such as DVDs and videos have higher fines, and that I am the only authorized user of this card.</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
   </si>
   <si>
     <t>confirm_note</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Please &lt;strong&gt;print this confirmation&lt;/strong&gt; and bring it with the following documents to any Oakland Public Library within 14 days to pick up your card:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Photo ID&lt;/li&gt;&lt;li&gt;Proof of address&lt;/li&gt;&lt;/ul&gt;&lt;p&gt; For children under 13, instead, a parent/Legal Guardian and child must both be present for the child to receive the card.&lt;/p&gt;</t>
   </si>
   <si>
     <t>button_print</t>
@@ -1209,6 +1203,57 @@
       </rPr>
       <t>而且明白本人是這張圖書証的唯一授權使用人。</t>
     </r>
+  </si>
+  <si>
+    <t>agreement_note_teen_adult</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Please &lt;strong&gt;print this confirmation&lt;/strong&gt; and bring it with the following documents to any Oakland Public Library within 14 days to pick up your card:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Photo ID&lt;/li&gt;&lt;li&gt;Proof of address&lt;/li&gt;&lt;/ul&gt;&lt;p&gt; For children under 13, a parent or legal guardian must be present with the child to receive the card. No ID or proof of address is required. &lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -2098,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,10 +2163,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2132,10 +2177,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2146,10 +2191,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2160,10 +2205,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2174,10 +2219,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2188,10 +2233,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2202,10 +2247,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2216,10 +2261,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2230,10 +2275,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,10 +2289,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,10 +2303,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2272,10 +2317,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="D12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2286,10 +2331,10 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>225</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2300,10 +2345,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,10 +2359,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2328,10 +2373,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2342,10 +2387,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2356,10 +2401,10 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>225</v>
+        <v>257</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2370,10 +2415,10 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
+        <v>258</v>
       </c>
       <c r="D19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2384,10 +2429,10 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2398,10 +2443,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D21" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2412,10 +2457,10 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2426,10 +2471,10 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2440,10 +2485,10 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2454,10 +2499,10 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2468,10 +2513,10 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2482,10 +2527,10 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2496,10 +2541,10 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2510,10 +2555,10 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2524,10 +2569,10 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2538,10 +2583,10 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2552,10 +2597,10 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2566,10 +2611,10 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2580,10 +2625,10 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2594,10 +2639,10 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2608,10 +2653,10 @@
         <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2622,10 +2667,10 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D37" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2636,10 +2681,10 @@
         <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2650,10 +2695,10 @@
         <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D39" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2664,10 +2709,10 @@
         <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2678,10 +2723,10 @@
         <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2692,10 +2737,10 @@
         <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2706,10 +2751,10 @@
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D43" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2720,10 +2765,10 @@
         <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D44" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2734,10 +2779,10 @@
         <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D45" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2748,10 +2793,10 @@
         <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D46" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2762,10 +2807,10 @@
         <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D47" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2776,10 +2821,10 @@
         <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D48" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2790,10 +2835,10 @@
         <v>97</v>
       </c>
       <c r="C49" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D49" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2804,10 +2849,10 @@
         <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D50" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2818,10 +2863,10 @@
         <v>101</v>
       </c>
       <c r="C51" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2832,10 +2877,10 @@
         <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D52" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2846,10 +2891,10 @@
         <v>105</v>
       </c>
       <c r="C53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D53" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2860,10 +2905,10 @@
         <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D54" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2874,374 +2919,374 @@
         <v>109</v>
       </c>
       <c r="C55" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D55" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" t="s">
         <v>110</v>
       </c>
-      <c r="B56" t="s">
-        <v>111</v>
-      </c>
       <c r="C56" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
         <v>113</v>
       </c>
-      <c r="B58" t="s">
-        <v>114</v>
-      </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D58" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D59" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" t="s">
         <v>116</v>
       </c>
-      <c r="B60" t="s">
-        <v>117</v>
-      </c>
       <c r="C60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" t="s">
         <v>118</v>
       </c>
-      <c r="B61" t="s">
-        <v>119</v>
-      </c>
       <c r="C61" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D61" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" t="s">
         <v>120</v>
       </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
       <c r="C62" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" t="s">
         <v>122</v>
       </c>
-      <c r="B63" t="s">
-        <v>123</v>
-      </c>
       <c r="C63" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
         <v>124</v>
       </c>
-      <c r="B64" t="s">
-        <v>125</v>
-      </c>
       <c r="C64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D64" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
         <v>126</v>
       </c>
-      <c r="B65" t="s">
-        <v>127</v>
-      </c>
       <c r="C65" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
         <v>128</v>
       </c>
-      <c r="B66" t="s">
-        <v>129</v>
-      </c>
       <c r="C66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D66" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" t="s">
         <v>130</v>
       </c>
-      <c r="B67" t="s">
-        <v>131</v>
-      </c>
       <c r="C67" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D67" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" t="s">
         <v>132</v>
       </c>
-      <c r="B68" t="s">
-        <v>133</v>
-      </c>
       <c r="C68" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D68" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>133</v>
+      </c>
+      <c r="B69" t="s">
         <v>134</v>
       </c>
-      <c r="B69" t="s">
-        <v>135</v>
-      </c>
       <c r="C69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>135</v>
+      </c>
+      <c r="B70" t="s">
         <v>136</v>
       </c>
-      <c r="B70" t="s">
-        <v>137</v>
-      </c>
       <c r="C70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" t="s">
         <v>138</v>
       </c>
-      <c r="B71" t="s">
-        <v>139</v>
-      </c>
       <c r="C71" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D71" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D72" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" t="s">
         <v>142</v>
       </c>
-      <c r="B74" t="s">
-        <v>143</v>
-      </c>
       <c r="C74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" t="s">
         <v>144</v>
       </c>
-      <c r="B75" t="s">
-        <v>145</v>
-      </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D75" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" t="s">
         <v>146</v>
       </c>
-      <c r="B76" t="s">
-        <v>147</v>
-      </c>
       <c r="C76" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
         <v>148</v>
       </c>
-      <c r="B77" t="s">
-        <v>149</v>
-      </c>
       <c r="C77" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D77" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" t="s">
         <v>150</v>
       </c>
-      <c r="B78" t="s">
-        <v>151</v>
-      </c>
       <c r="C78" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D78" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>260</v>
       </c>
       <c r="C79" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D79" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D80" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ident_note chinese text
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -709,9 +709,6 @@
     <t>家長/法定監護人資料</t>
   </si>
   <si>
-    <t xml:space="preserve">你可選擇使用任何一種身份証明文件申請圖書証。請點擊以下按鈕，然後輸入証件上的號碼。有關可接受的身份証種類詳情，請參閱 </t>
-  </si>
-  <si>
     <t xml:space="preserve">駕駛執照 </t>
   </si>
   <si>
@@ -1027,6 +1024,9 @@
   </si>
   <si>
     <t>Favor de Indicar su Fecha de Nacimiento</t>
+  </si>
+  <si>
+    <t>你可選擇使用任何一種身份証明文件申請圖書証。請點擊以下按鈕，然後輸入証件上的號碼。若你所持的証件這裡没有列出，請向圖書館職員查詢。</t>
   </si>
 </sst>
 </file>
@@ -1882,14 +1882,14 @@
   <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="76.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="58.28515625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -1916,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D2" t="s">
         <v>159</v>
@@ -1930,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D3" t="s">
         <v>220</v>
@@ -1944,7 +1944,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D4" t="s">
         <v>181</v>
@@ -1958,10 +1958,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D6" t="s">
         <v>197</v>
@@ -1986,7 +1986,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D7" t="s">
         <v>185</v>
@@ -2000,7 +2000,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D8" t="s">
         <v>186</v>
@@ -2014,7 +2014,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D9" t="s">
         <v>187</v>
@@ -2028,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D10" t="s">
         <v>188</v>
@@ -2042,7 +2042,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D11" t="s">
         <v>189</v>
@@ -2056,7 +2056,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
         <v>190</v>
@@ -2070,7 +2070,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D13" t="s">
         <v>191</v>
@@ -2084,7 +2084,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D14" t="s">
         <v>192</v>
@@ -2098,7 +2098,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D15" t="s">
         <v>193</v>
@@ -2112,7 +2112,7 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
         <v>194</v>
@@ -2126,7 +2126,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
         <v>195</v>
@@ -2140,7 +2140,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D18" t="s">
         <v>196</v>
@@ -2154,7 +2154,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D19" t="s">
         <v>198</v>
@@ -2168,7 +2168,7 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D20" t="s">
         <v>199</v>
@@ -2182,7 +2182,7 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D21" t="s">
         <v>221</v>
@@ -2196,7 +2196,7 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D22" t="s">
         <v>180</v>
@@ -2210,7 +2210,7 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D23" t="s">
         <v>160</v>
@@ -2224,7 +2224,7 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D24" t="s">
         <v>222</v>
@@ -2238,10 +2238,10 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,10 +2252,10 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D27" t="s">
         <v>161</v>
@@ -2280,7 +2280,7 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
         <v>162</v>
@@ -2294,7 +2294,7 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D29" t="s">
         <v>163</v>
@@ -2308,7 +2308,7 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D30" t="s">
         <v>164</v>
@@ -2322,7 +2322,7 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D31" t="s">
         <v>165</v>
@@ -2336,7 +2336,7 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D32" t="s">
         <v>166</v>
@@ -2350,7 +2350,7 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D33" t="s">
         <v>167</v>
@@ -2364,7 +2364,7 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D34" t="s">
         <v>168</v>
@@ -2378,7 +2378,7 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D35" t="s">
         <v>169</v>
@@ -2392,7 +2392,7 @@
         <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D36" t="s">
         <v>170</v>
@@ -2406,7 +2406,7 @@
         <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D37" t="s">
         <v>223</v>
@@ -2414,13 +2414,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s">
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D38" t="s">
         <v>167</v>
@@ -2428,13 +2428,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D39" t="s">
         <v>168</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s">
         <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D40" t="s">
         <v>169</v>
@@ -2456,13 +2456,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s">
         <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D41" t="s">
         <v>170</v>
@@ -2476,7 +2476,7 @@
         <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D42" t="s">
         <v>171</v>
@@ -2490,7 +2490,7 @@
         <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D43" t="s">
         <v>172</v>
@@ -2504,7 +2504,7 @@
         <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D44" t="s">
         <v>173</v>
@@ -2518,7 +2518,7 @@
         <v>81</v>
       </c>
       <c r="C45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D45" t="s">
         <v>174</v>
@@ -2532,7 +2532,7 @@
         <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D46" t="s">
         <v>175</v>
@@ -2546,7 +2546,7 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D47" t="s">
         <v>224</v>
@@ -2560,7 +2560,7 @@
         <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D48" t="s">
         <v>182</v>
@@ -2574,7 +2574,7 @@
         <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D49" t="s">
         <v>176</v>
@@ -2588,10 +2588,10 @@
         <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D50" t="s">
-        <v>225</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,10 +2602,10 @@
         <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2616,10 +2616,10 @@
         <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2630,10 +2630,10 @@
         <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2644,10 +2644,10 @@
         <v>99</v>
       </c>
       <c r="C54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D54" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2658,10 +2658,10 @@
         <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,10 +2672,10 @@
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D56" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,10 +2686,10 @@
         <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D57" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2700,7 +2700,7 @@
         <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D58" t="s">
         <v>177</v>
@@ -2714,7 +2714,7 @@
         <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D59" t="s">
         <v>178</v>
@@ -2722,16 +2722,16 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B60" t="s">
         <v>110</v>
       </c>
       <c r="C60" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D60" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2742,7 +2742,7 @@
         <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D61" t="s">
         <v>183</v>
@@ -2756,7 +2756,7 @@
         <v>113</v>
       </c>
       <c r="C62" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D62" t="s">
         <v>179</v>
@@ -2770,7 +2770,7 @@
         <v>157</v>
       </c>
       <c r="C63" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D63" t="s">
         <v>203</v>
@@ -2784,7 +2784,7 @@
         <v>116</v>
       </c>
       <c r="C64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D64" t="s">
         <v>202</v>
@@ -2798,7 +2798,7 @@
         <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D65" t="s">
         <v>215</v>
@@ -2812,7 +2812,7 @@
         <v>120</v>
       </c>
       <c r="C66" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D66" t="s">
         <v>216</v>
@@ -2826,7 +2826,7 @@
         <v>122</v>
       </c>
       <c r="C67" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D67" t="s">
         <v>201</v>
@@ -2840,7 +2840,7 @@
         <v>124</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D68" t="s">
         <v>205</v>
@@ -2854,7 +2854,7 @@
         <v>126</v>
       </c>
       <c r="C69" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D69" t="s">
         <v>206</v>
@@ -2868,7 +2868,7 @@
         <v>128</v>
       </c>
       <c r="C70" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D70" t="s">
         <v>207</v>
@@ -2882,7 +2882,7 @@
         <v>130</v>
       </c>
       <c r="C71" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D71" t="s">
         <v>208</v>
@@ -2896,7 +2896,7 @@
         <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D72" t="s">
         <v>217</v>
@@ -2910,7 +2910,7 @@
         <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D73" t="s">
         <v>209</v>
@@ -2924,7 +2924,7 @@
         <v>136</v>
       </c>
       <c r="C74" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D74" t="s">
         <v>210</v>
@@ -2938,7 +2938,7 @@
         <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D75" t="s">
         <v>211</v>
@@ -2952,7 +2952,7 @@
         <v>132</v>
       </c>
       <c r="C76" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D76" t="s">
         <v>217</v>
@@ -2966,7 +2966,7 @@
         <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D77" t="s">
         <v>212</v>
@@ -2980,7 +2980,7 @@
         <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D78" t="s">
         <v>213</v>
@@ -2994,7 +2994,7 @@
         <v>144</v>
       </c>
       <c r="C79" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D79" t="s">
         <v>218</v>
@@ -3008,7 +3008,7 @@
         <v>146</v>
       </c>
       <c r="C80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D80" t="s">
         <v>200</v>
@@ -3022,7 +3022,7 @@
         <v>148</v>
       </c>
       <c r="C81" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D81" t="s">
         <v>214</v>
@@ -3036,7 +3036,7 @@
         <v>150</v>
       </c>
       <c r="C82" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D82" t="s">
         <v>204</v>
@@ -3050,10 +3050,10 @@
         <v>152</v>
       </c>
       <c r="C83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D83" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>154</v>
       </c>
       <c r="C84" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D84" t="s">
         <v>219</v>
@@ -3075,13 +3075,13 @@
         <v>184</v>
       </c>
       <c r="B85" t="s">
+        <v>319</v>
+      </c>
+      <c r="C85" t="s">
         <v>320</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>321</v>
-      </c>
-      <c r="D85" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
submit button now has unique id in selfreg.html
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="token_data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="token_data" localSheetId="0">token_data!$A$1:$D$85</definedName>
+    <definedName name="token_data" localSheetId="0">token_data!$A$1:$D$86</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="325">
   <si>
     <t>header</t>
   </si>
@@ -1027,6 +1027,9 @@
   </si>
   <si>
     <t>你可選擇使用任何一種身份証明文件申請圖書証。請點擊以下按鈕，然後輸入証件上的號碼。若你所持的証件這裡没有列出，請向圖書館職員查詢。</t>
+  </si>
+  <si>
+    <t>submit_age</t>
   </si>
 </sst>
 </file>
@@ -1879,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2179,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>324</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
@@ -2190,897 +2193,911 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D24" t="s">
-        <v>222</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D25" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D26" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D27" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>300</v>
+        <v>247</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
       <c r="D34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>296</v>
+        <v>249</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D37" t="s">
-        <v>223</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>276</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D38" t="s">
-        <v>167</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
       <c r="D39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>296</v>
+        <v>249</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>279</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>313</v>
+        <v>252</v>
       </c>
       <c r="D47" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>253</v>
+        <v>313</v>
       </c>
       <c r="D48" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>314</v>
+        <v>253</v>
       </c>
       <c r="D49" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>254</v>
+        <v>314</v>
       </c>
       <c r="D50" t="s">
-        <v>323</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>315</v>
+        <v>254</v>
       </c>
       <c r="D51" t="s">
-        <v>225</v>
+        <v>323</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D53" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D54" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>255</v>
+        <v>318</v>
       </c>
       <c r="D55" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>306</v>
+        <v>255</v>
       </c>
       <c r="D56" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>256</v>
+        <v>306</v>
       </c>
       <c r="D57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>305</v>
+        <v>256</v>
       </c>
       <c r="D58" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>236</v>
+        <v>108</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>257</v>
+        <v>304</v>
       </c>
       <c r="D60" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>111</v>
+        <v>236</v>
       </c>
       <c r="B61" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D62" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="C63" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="D63" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="C64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D64" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>260</v>
+        <v>312</v>
       </c>
       <c r="D65" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C66" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="D66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B67" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C67" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D72" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D73" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D74" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B76" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C76" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D76" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C77" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D77" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C78" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D79" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="D80" t="s">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C81" t="s">
-        <v>273</v>
+        <v>308</v>
       </c>
       <c r="D81" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C82" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
       <c r="D82" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C83" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="D84" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>153</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C85" t="s">
+        <v>307</v>
+      </c>
+      <c r="D85" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>184</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>319</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>320</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>321</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated chinese translations for some strings
</commit_message>
<xml_diff>
--- a/token_data.xlsx
+++ b/token_data.xlsx
@@ -583,9 +583,6 @@
     <t>學校</t>
   </si>
   <si>
-    <t>作為家長/監護人我明白及同意&lt;br/&gt;&lt;ul&gt;&lt;li&gt;圖書館只發証給我的孩子，只有我的孩子才能使用這張圖書証。&lt;/li&gt;&lt;li&gt;圖書館容許孩子從任何部份借出任何物件。即使在本人的要求下，圖書館不能限制孩子借出書本及電影的種類。&lt;/li&gt;&lt;li&gt;孩子的資料保密與本人一樣是受加州私隱權法例保障的。圖書館不可向我透露孩子借出的任何資料，除物件有罰款以外。&lt;/li&gt;&lt;li&gt;某些圖書館物件是有過期罰款的。所有遺失及損壞物件均需繳付費用。本人同意對孩子借出的一切物件負責，並擔負所有過期罰款及任何損壞費用。&lt;/li&gt;&lt;li&gt;我的孩子每天只可在圖書館內使用不超過一小時的電腦 圖書館不會監察孩子在網上查閱的任何資料。&lt;/li&gt;&lt;li&gt;若我的孩子年齡是八歲以下，必須時刻由家長或保姆監督，絶不可以單獨逗留在圖書館內。&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>button_close</t>
   </si>
   <si>
@@ -859,32 +856,6 @@
     <t>&lt;p&gt;Favor de&lt;strong&gt;imprimir esta confirmación&lt;/strong&gt; y llévela con sus documentos cualquier sucursal de la Biblioteca Publica de Oakland durante los próximos 14 días para recibir su tarjeta:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Identificación con foto&lt;/li&gt;&lt;li&gt;Prueba de domicilio&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Niños menores de 13 años de edad, el padre/guardian y el niño tiene que estar presente para recibir la tarjeta. &lt;/p&gt;</t>
   </si>
   <si>
-    <r>
-      <t>家長/法定監護人和孩子在填寫申請表格後十四日內，必須一同前往圖書館領取孩子的圖書証。家長/法定監護人亦可預先填寫&lt;a href="http://www.oaklandlibrary.org/sites/default/files/uploads/OPL_Card_App_Eng_Kids_0.pdf"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>書面申請表格&lt;/a&gt;，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>讓孩子在沒有家表的陪同下仍可辨理申請手續。</t>
-    </r>
-  </si>
-  <si>
     <t>mailing_street</t>
   </si>
   <si>
@@ -1030,6 +1001,12 @@
   </si>
   <si>
     <t>submit_age</t>
+  </si>
+  <si>
+    <t>家長/法定監護人和孩子在填寫申請表格後十四日內，必須一同前往圖書館領取孩子的圖書証。家長/法定監護人亦可預先填寫&lt;a href="http://www.oaklandlibrary.org/sites/default/files/uploads/OPL_Card_App_Eng_Kids_0.pdf"&gt;書面申請表格&lt;/a&gt;，讓孩子在沒有家長的陪同下仍可辨理申請手續。</t>
+  </si>
+  <si>
+    <t>作為家長/監護人我明白及同意&lt;br/&gt;&lt;ul&gt;&lt;li&gt;圖書館只發証給我的孩子，只有我的孩子才能使用這張圖書証。&lt;/li&gt;&lt;li&gt;圖書館容許孩子從任何部份借出任何物件。即使在本人的要求下，圖書館不能限制孩子借出書本及電影的種類。&lt;/li&gt;&lt;li&gt;孩子的資料保密與本人一樣是受加州私隱權法例保障的。除物件有罰款以外, 圖書館不可向我透露孩子借出的任何資料。&lt;/li&gt;&lt;li&gt;某些圖書館物件是有過期罰款的。所有遺失及損壞物件均需繳付費用。本人同意對孩子借出的一切物件負責，並擔負所有過期罰款及任何損壞費用。&lt;/li&gt;&lt;li&gt;我的孩子每天只可在圖書館內使用不超過一小時的電腦。圖書館不會監察孩子在網上查閱的任何資料。&lt;/li&gt;&lt;li&gt;若我的孩子年齡是八歲以下，必須時刻由家長或保姆監督，絶不可以單獨逗留在圖書館內。&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1919,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D2" t="s">
         <v>159</v>
@@ -1933,10 +1910,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1947,7 +1924,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D4" t="s">
         <v>181</v>
@@ -1961,10 +1938,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,10 +1952,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1989,10 +1966,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2003,10 +1980,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2017,10 +1994,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2031,10 +2008,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2045,10 +2022,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2059,10 +2036,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,10 +2050,10 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2087,10 +2064,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,10 +2078,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2115,10 +2092,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2129,10 +2106,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2143,10 +2120,10 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2157,10 +2134,10 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2171,24 +2148,24 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2199,10 +2176,10 @@
         <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2213,7 +2190,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D23" t="s">
         <v>180</v>
@@ -2227,7 +2204,7 @@
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D24" t="s">
         <v>160</v>
@@ -2241,10 +2218,10 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2255,10 +2232,10 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2269,10 +2246,10 @@
         <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D27" t="s">
-        <v>275</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2283,7 +2260,7 @@
         <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D28" t="s">
         <v>161</v>
@@ -2297,7 +2274,7 @@
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D29" t="s">
         <v>162</v>
@@ -2311,7 +2288,7 @@
         <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D30" t="s">
         <v>163</v>
@@ -2325,7 +2302,7 @@
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D31" t="s">
         <v>164</v>
@@ -2339,7 +2316,7 @@
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D32" t="s">
         <v>165</v>
@@ -2353,7 +2330,7 @@
         <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D33" t="s">
         <v>166</v>
@@ -2367,7 +2344,7 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D34" t="s">
         <v>167</v>
@@ -2381,7 +2358,7 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D35" t="s">
         <v>168</v>
@@ -2395,7 +2372,7 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D36" t="s">
         <v>169</v>
@@ -2409,7 +2386,7 @@
         <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D37" t="s">
         <v>170</v>
@@ -2423,21 +2400,21 @@
         <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B39" t="s">
         <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D39" t="s">
         <v>167</v>
@@ -2445,13 +2422,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D40" t="s">
         <v>168</v>
@@ -2459,13 +2436,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B41" t="s">
         <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D41" t="s">
         <v>169</v>
@@ -2473,13 +2450,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B42" t="s">
         <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D42" t="s">
         <v>170</v>
@@ -2493,7 +2470,7 @@
         <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D43" t="s">
         <v>171</v>
@@ -2507,7 +2484,7 @@
         <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D44" t="s">
         <v>172</v>
@@ -2521,7 +2498,7 @@
         <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D45" t="s">
         <v>173</v>
@@ -2535,7 +2512,7 @@
         <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D46" t="s">
         <v>174</v>
@@ -2549,7 +2526,7 @@
         <v>83</v>
       </c>
       <c r="C47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" t="s">
         <v>175</v>
@@ -2563,10 +2540,10 @@
         <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,7 +2554,7 @@
         <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D49" t="s">
         <v>182</v>
@@ -2591,7 +2568,7 @@
         <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D50" t="s">
         <v>176</v>
@@ -2605,10 +2582,10 @@
         <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D51" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2619,10 +2596,10 @@
         <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D52" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,10 +2610,10 @@
         <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2647,10 +2624,10 @@
         <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2661,10 +2638,10 @@
         <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2675,10 +2652,10 @@
         <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D56" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2689,10 +2666,10 @@
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D57" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2703,10 +2680,10 @@
         <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,7 +2694,7 @@
         <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D59" t="s">
         <v>177</v>
@@ -2731,7 +2708,7 @@
         <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D60" t="s">
         <v>178</v>
@@ -2739,16 +2716,16 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B61" t="s">
         <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2759,10 +2736,10 @@
         <v>156</v>
       </c>
       <c r="C62" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D62" t="s">
-        <v>183</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2773,7 +2750,7 @@
         <v>113</v>
       </c>
       <c r="C63" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D63" t="s">
         <v>179</v>
@@ -2787,10 +2764,10 @@
         <v>157</v>
       </c>
       <c r="C64" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,10 +2778,10 @@
         <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,10 +2792,10 @@
         <v>118</v>
       </c>
       <c r="C66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2829,10 +2806,10 @@
         <v>120</v>
       </c>
       <c r="C67" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2843,10 +2820,10 @@
         <v>122</v>
       </c>
       <c r="C68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2857,10 +2834,10 @@
         <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D69" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2871,10 +2848,10 @@
         <v>126</v>
       </c>
       <c r="C70" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2885,10 +2862,10 @@
         <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D71" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2899,10 +2876,10 @@
         <v>130</v>
       </c>
       <c r="C72" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2913,10 +2890,10 @@
         <v>132</v>
       </c>
       <c r="C73" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2927,10 +2904,10 @@
         <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2941,10 +2918,10 @@
         <v>136</v>
       </c>
       <c r="C75" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2955,10 +2932,10 @@
         <v>138</v>
       </c>
       <c r="C76" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2969,10 +2946,10 @@
         <v>132</v>
       </c>
       <c r="C77" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2983,10 +2960,10 @@
         <v>134</v>
       </c>
       <c r="C78" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2997,10 +2974,10 @@
         <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D79" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3011,10 +2988,10 @@
         <v>144</v>
       </c>
       <c r="C80" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3025,10 +3002,10 @@
         <v>146</v>
       </c>
       <c r="C81" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,10 +3016,10 @@
         <v>148</v>
       </c>
       <c r="C82" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3053,10 +3030,10 @@
         <v>150</v>
       </c>
       <c r="C83" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D83" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3067,10 +3044,10 @@
         <v>152</v>
       </c>
       <c r="C84" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D84" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3081,24 +3058,24 @@
         <v>154</v>
       </c>
       <c r="C85" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B86" t="s">
+        <v>317</v>
+      </c>
+      <c r="C86" t="s">
+        <v>318</v>
+      </c>
+      <c r="D86" t="s">
         <v>319</v>
-      </c>
-      <c r="C86" t="s">
-        <v>320</v>
-      </c>
-      <c r="D86" t="s">
-        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>